<commit_message>
analysis of IT-caregiver data
</commit_message>
<xml_diff>
--- a/7 Final Item Sets FEB 2019/SPM-2_Infant-Toddler_Items_FINAL.xlsx
+++ b/7 Final Item Sets FEB 2019/SPM-2_Infant-Toddler_Items_FINAL.xlsx
@@ -8,41 +8,46 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dherzberg/Desktop/SPM2-R/7 Final Item Sets FEB 2019/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9580F928-630E-5D45-84C5-3B11AD6F9169}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBC3200F-8F43-D145-BC7B-B1D8569D4620}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="28800" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="28340" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="4-9" sheetId="1" r:id="rId1"/>
     <sheet name="10-30" sheetId="4" r:id="rId2"/>
-    <sheet name="49 Caregiver" sheetId="3" r:id="rId3"/>
-    <sheet name="1030 Caregiver" sheetId="7" r:id="rId4"/>
-    <sheet name="DELETED ITEMS" sheetId="5" r:id="rId5"/>
-    <sheet name="Scratch" sheetId="8" r:id="rId6"/>
+    <sheet name="Caregiver" sheetId="9" r:id="rId3"/>
+    <sheet name="49 Caregiver" sheetId="3" r:id="rId4"/>
+    <sheet name="1030 Caregiver" sheetId="7" r:id="rId5"/>
+    <sheet name="DELETED ITEMS" sheetId="5" r:id="rId6"/>
+    <sheet name="Scratch" sheetId="8" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'10-30'!$A$1:$G$81</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'1030 Caregiver'!$A$1:$G$81</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'1030 Caregiver'!$A$1:$G$81</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'4-9'!$A$1:$G$81</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'49 Caregiver'!$A$1:$G$81</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'49 Caregiver'!$A$1:$G$81</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Caregiver!$A$1:$G$81</definedName>
     <definedName name="Z_3D544592_D893_4912_8A4C_A9212B9C1328_.wvu.FilterData" localSheetId="1" hidden="1">'10-30'!$A$1:$G$81</definedName>
-    <definedName name="Z_3D544592_D893_4912_8A4C_A9212B9C1328_.wvu.FilterData" localSheetId="3" hidden="1">'1030 Caregiver'!$A$1:$G$81</definedName>
+    <definedName name="Z_3D544592_D893_4912_8A4C_A9212B9C1328_.wvu.FilterData" localSheetId="4" hidden="1">'1030 Caregiver'!$A$1:$G$81</definedName>
     <definedName name="Z_3D544592_D893_4912_8A4C_A9212B9C1328_.wvu.FilterData" localSheetId="0" hidden="1">'4-9'!$A$1:$G$81</definedName>
-    <definedName name="Z_3D544592_D893_4912_8A4C_A9212B9C1328_.wvu.FilterData" localSheetId="2" hidden="1">'49 Caregiver'!$A$1:$G$81</definedName>
+    <definedName name="Z_3D544592_D893_4912_8A4C_A9212B9C1328_.wvu.FilterData" localSheetId="3" hidden="1">'49 Caregiver'!$A$1:$G$81</definedName>
+    <definedName name="Z_3D544592_D893_4912_8A4C_A9212B9C1328_.wvu.FilterData" localSheetId="2" hidden="1">Caregiver!$A$1:$G$81</definedName>
     <definedName name="Z_7283F7E0_0B2D_4F5B_B955_ADB97BAFC841_.wvu.FilterData" localSheetId="1" hidden="1">'10-30'!$A$1:$G$81</definedName>
-    <definedName name="Z_7283F7E0_0B2D_4F5B_B955_ADB97BAFC841_.wvu.FilterData" localSheetId="3" hidden="1">'1030 Caregiver'!$A$1:$G$81</definedName>
+    <definedName name="Z_7283F7E0_0B2D_4F5B_B955_ADB97BAFC841_.wvu.FilterData" localSheetId="4" hidden="1">'1030 Caregiver'!$A$1:$G$81</definedName>
     <definedName name="Z_7283F7E0_0B2D_4F5B_B955_ADB97BAFC841_.wvu.FilterData" localSheetId="0" hidden="1">'4-9'!$A$1:$G$81</definedName>
-    <definedName name="Z_7283F7E0_0B2D_4F5B_B955_ADB97BAFC841_.wvu.FilterData" localSheetId="2" hidden="1">'49 Caregiver'!$A$1:$G$81</definedName>
+    <definedName name="Z_7283F7E0_0B2D_4F5B_B955_ADB97BAFC841_.wvu.FilterData" localSheetId="3" hidden="1">'49 Caregiver'!$A$1:$G$81</definedName>
+    <definedName name="Z_7283F7E0_0B2D_4F5B_B955_ADB97BAFC841_.wvu.FilterData" localSheetId="2" hidden="1">Caregiver!$A$1:$G$81</definedName>
     <definedName name="Z_E395C88E_3BA8_B344_A1BC_A46BF8755BD3_.wvu.Cols" localSheetId="1" hidden="1">'10-30'!$C:$C</definedName>
-    <definedName name="Z_E395C88E_3BA8_B344_A1BC_A46BF8755BD3_.wvu.Cols" localSheetId="3" hidden="1">'1030 Caregiver'!$C:$C</definedName>
+    <definedName name="Z_E395C88E_3BA8_B344_A1BC_A46BF8755BD3_.wvu.Cols" localSheetId="4" hidden="1">'1030 Caregiver'!$C:$C</definedName>
     <definedName name="Z_E395C88E_3BA8_B344_A1BC_A46BF8755BD3_.wvu.Cols" localSheetId="0" hidden="1">'4-9'!$C:$C</definedName>
-    <definedName name="Z_E395C88E_3BA8_B344_A1BC_A46BF8755BD3_.wvu.Cols" localSheetId="2" hidden="1">'49 Caregiver'!$C:$C</definedName>
+    <definedName name="Z_E395C88E_3BA8_B344_A1BC_A46BF8755BD3_.wvu.Cols" localSheetId="3" hidden="1">'49 Caregiver'!$C:$C</definedName>
+    <definedName name="Z_E395C88E_3BA8_B344_A1BC_A46BF8755BD3_.wvu.Cols" localSheetId="2" hidden="1">Caregiver!$C:$C</definedName>
   </definedNames>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <customWorkbookViews>
+    <customWorkbookView name="Microsoft Office User - Personal View" guid="{E395C88E-3BA8-B344-A1BC-A46BF8755BD3}" mergeInterval="0" personalView="1" minimized="1" windowWidth="0" windowHeight="0" activeSheetId="2"/>
+    <customWorkbookView name="XXXXX - Personal View" guid="{7283F7E0-0B2D-4F5B-B955-ADB97BAFC841}" mergeInterval="0" personalView="1" xWindow="52" yWindow="74" windowWidth="1858" windowHeight="946" activeSheetId="1"/>
     <customWorkbookView name="John Williams - Personal View" guid="{3D544592-D893-4912-8A4C-A9212B9C1328}" mergeInterval="0" personalView="1" maximized="1" xWindow="1672" yWindow="-8" windowWidth="1696" windowHeight="1066" activeSheetId="2"/>
-    <customWorkbookView name="XXXXX - Personal View" guid="{7283F7E0-0B2D-4F5B-B955-ADB97BAFC841}" mergeInterval="0" personalView="1" xWindow="52" yWindow="74" windowWidth="1858" windowHeight="946" activeSheetId="1"/>
-    <customWorkbookView name="Microsoft Office User - Personal View" guid="{E395C88E-3BA8-B344-A1BC-A46BF8755BD3}" mergeInterval="0" personalView="1" minimized="1" windowWidth="0" windowHeight="0" activeSheetId="2"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -62,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1865" uniqueCount="542">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2208" uniqueCount="622">
   <si>
     <t>REF</t>
   </si>
@@ -1741,14 +1746,261 @@
   <si>
     <t>q0236</t>
   </si>
+  <si>
+    <t>QT108</t>
+  </si>
+  <si>
+    <t>QT107</t>
+  </si>
+  <si>
+    <t>QT106</t>
+  </si>
+  <si>
+    <t>QT105</t>
+  </si>
+  <si>
+    <t>QT103</t>
+  </si>
+  <si>
+    <t>QT101</t>
+  </si>
+  <si>
+    <t>QT100</t>
+  </si>
+  <si>
+    <t>QT98</t>
+  </si>
+  <si>
+    <t>QT97</t>
+  </si>
+  <si>
+    <t>QT96</t>
+  </si>
+  <si>
+    <t>QT95</t>
+  </si>
+  <si>
+    <t>QT94</t>
+  </si>
+  <si>
+    <t>QT93</t>
+  </si>
+  <si>
+    <t>QT92</t>
+  </si>
+  <si>
+    <t>QT91</t>
+  </si>
+  <si>
+    <t>QT89</t>
+  </si>
+  <si>
+    <t>QT87</t>
+  </si>
+  <si>
+    <t>QT86</t>
+  </si>
+  <si>
+    <t>QT85</t>
+  </si>
+  <si>
+    <t>QT83</t>
+  </si>
+  <si>
+    <t>QT81</t>
+  </si>
+  <si>
+    <t>QT79</t>
+  </si>
+  <si>
+    <t>QT78</t>
+  </si>
+  <si>
+    <t>QT77</t>
+  </si>
+  <si>
+    <t>QT76</t>
+  </si>
+  <si>
+    <t>QT75</t>
+  </si>
+  <si>
+    <t>QT74</t>
+  </si>
+  <si>
+    <t>QT73</t>
+  </si>
+  <si>
+    <t>QT72</t>
+  </si>
+  <si>
+    <t>QT71</t>
+  </si>
+  <si>
+    <t>QT69</t>
+  </si>
+  <si>
+    <t>QT68</t>
+  </si>
+  <si>
+    <t>QT67</t>
+  </si>
+  <si>
+    <t>QT66</t>
+  </si>
+  <si>
+    <t>QT65</t>
+  </si>
+  <si>
+    <t>QT62</t>
+  </si>
+  <si>
+    <t>QT60</t>
+  </si>
+  <si>
+    <t>QT57</t>
+  </si>
+  <si>
+    <t>QT56</t>
+  </si>
+  <si>
+    <t>QT55</t>
+  </si>
+  <si>
+    <t>QT54</t>
+  </si>
+  <si>
+    <t>QT51</t>
+  </si>
+  <si>
+    <t>QT50</t>
+  </si>
+  <si>
+    <t>QT49</t>
+  </si>
+  <si>
+    <t>QT48</t>
+  </si>
+  <si>
+    <t>QT47</t>
+  </si>
+  <si>
+    <t>QT46</t>
+  </si>
+  <si>
+    <t>QT45</t>
+  </si>
+  <si>
+    <t>QT43</t>
+  </si>
+  <si>
+    <t>QT41</t>
+  </si>
+  <si>
+    <t>QT39</t>
+  </si>
+  <si>
+    <t>QT37</t>
+  </si>
+  <si>
+    <t>QT35</t>
+  </si>
+  <si>
+    <t>QT34</t>
+  </si>
+  <si>
+    <t>QT33</t>
+  </si>
+  <si>
+    <t>QT32</t>
+  </si>
+  <si>
+    <t>QT31</t>
+  </si>
+  <si>
+    <t>QT30</t>
+  </si>
+  <si>
+    <t>QT28</t>
+  </si>
+  <si>
+    <t>QT27</t>
+  </si>
+  <si>
+    <t>QT26</t>
+  </si>
+  <si>
+    <t>QT25</t>
+  </si>
+  <si>
+    <t>QT23</t>
+  </si>
+  <si>
+    <t>QT21</t>
+  </si>
+  <si>
+    <t>QT20</t>
+  </si>
+  <si>
+    <t>QT19</t>
+  </si>
+  <si>
+    <t>QT18</t>
+  </si>
+  <si>
+    <t>QT17</t>
+  </si>
+  <si>
+    <t>QT15</t>
+  </si>
+  <si>
+    <t>QT14</t>
+  </si>
+  <si>
+    <t>QT13</t>
+  </si>
+  <si>
+    <t>QT12</t>
+  </si>
+  <si>
+    <t>QT11</t>
+  </si>
+  <si>
+    <t>QT10</t>
+  </si>
+  <si>
+    <t>QT7</t>
+  </si>
+  <si>
+    <t>QT6</t>
+  </si>
+  <si>
+    <t>QT5</t>
+  </si>
+  <si>
+    <t>QT4</t>
+  </si>
+  <si>
+    <t>QT2</t>
+  </si>
+  <si>
+    <t>QT1</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="16">
+  <fonts count="17">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -2023,13 +2275,13 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="138">
+  <cellXfs count="141">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -2038,34 +2290,34 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2074,307 +2326,312 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="2" fontId="11" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="12" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="2" fontId="11" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="12" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="2" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="2" fontId="13" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="14" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="2" fontId="11" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="12" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="2" fontId="11" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="12" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -4458,11 +4715,10 @@
     <sortCondition sortBy="cellColor" ref="G2:G111" dxfId="2"/>
   </sortState>
   <customSheetViews>
-    <customSheetView guid="{3D544592-D893-4912-8A4C-A9212B9C1328}" fitToPage="1">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="G1" sqref="G1:L1048576"/>
+    <customSheetView guid="{E395C88E-3BA8-B344-A1BC-A46BF8755BD3}" fitToPage="1" hiddenColumns="1" topLeftCell="A55">
+      <selection activeCell="F78" sqref="F78"/>
       <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
-      <pageSetup scale="80" fitToHeight="4" orientation="landscape" r:id="rId1"/>
+      <pageSetup scale="64" fitToHeight="4" orientation="landscape" r:id="rId1"/>
     </customSheetView>
     <customSheetView guid="{7283F7E0-0B2D-4F5B-B955-ADB97BAFC841}" fitToPage="1" showAutoFilter="1">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
@@ -4475,13 +4731,14 @@
         </sortState>
       </autoFilter>
     </customSheetView>
-    <customSheetView guid="{E395C88E-3BA8-B344-A1BC-A46BF8755BD3}" fitToPage="1" hiddenColumns="1" topLeftCell="A55">
-      <selection activeCell="F78" sqref="F78"/>
+    <customSheetView guid="{3D544592-D893-4912-8A4C-A9212B9C1328}" fitToPage="1">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="G1" sqref="G1:L1048576"/>
       <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
-      <pageSetup scale="64" fitToHeight="4" orientation="landscape" r:id="rId3"/>
+      <pageSetup scale="80" fitToHeight="4" orientation="landscape" r:id="rId3"/>
     </customSheetView>
   </customSheetViews>
-  <phoneticPr fontId="7" type="noConversion"/>
+  <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="80" fitToHeight="4" orientation="landscape" r:id="rId4"/>
 </worksheet>
@@ -6264,6 +6521,1771 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9257C3D-DA87-A847-8AB9-4C5885F608C5}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:G81"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="186" zoomScaleNormal="75" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A28" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="G1" sqref="G1:G1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="5.6640625" style="31" customWidth="1"/>
+    <col min="2" max="2" width="5.6640625" style="39" customWidth="1"/>
+    <col min="3" max="3" width="7.5" style="26" customWidth="1"/>
+    <col min="4" max="4" width="5.6640625" style="39" customWidth="1"/>
+    <col min="5" max="5" width="5.6640625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="10.5" style="3" customWidth="1"/>
+    <col min="7" max="7" width="86.5" style="55" customWidth="1"/>
+    <col min="8" max="16384" width="8.83203125" style="31"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" s="131" customFormat="1" ht="18" thickBot="1">
+      <c r="A1" s="101" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="102" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="103" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="104" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="105" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="106" t="s">
+        <v>294</v>
+      </c>
+      <c r="G1" s="107" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="17">
+      <c r="A2" s="127">
+        <v>1</v>
+      </c>
+      <c r="B2" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="109" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="33" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="24">
+        <v>1</v>
+      </c>
+      <c r="F2" s="70" t="s">
+        <v>621</v>
+      </c>
+      <c r="G2" s="51" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="17">
+      <c r="A3" s="128">
+        <v>2</v>
+      </c>
+      <c r="B3" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="75" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="21">
+        <v>2</v>
+      </c>
+      <c r="F3" s="68" t="s">
+        <v>620</v>
+      </c>
+      <c r="G3" s="52" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="17">
+      <c r="A4" s="128">
+        <v>4</v>
+      </c>
+      <c r="B4" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="75" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="21">
+        <v>4</v>
+      </c>
+      <c r="F4" s="68" t="s">
+        <v>619</v>
+      </c>
+      <c r="G4" s="52" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="17">
+      <c r="A5" s="128">
+        <v>5</v>
+      </c>
+      <c r="B5" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="75" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="21">
+        <v>5</v>
+      </c>
+      <c r="F5" s="68" t="s">
+        <v>618</v>
+      </c>
+      <c r="G5" s="52" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="17">
+      <c r="A6" s="128">
+        <v>6</v>
+      </c>
+      <c r="B6" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="75" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="21">
+        <v>6</v>
+      </c>
+      <c r="F6" s="68" t="s">
+        <v>617</v>
+      </c>
+      <c r="G6" s="52" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="17">
+      <c r="A7" s="128">
+        <v>7</v>
+      </c>
+      <c r="B7" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="75" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="21">
+        <v>7</v>
+      </c>
+      <c r="F7" s="68" t="s">
+        <v>616</v>
+      </c>
+      <c r="G7" s="52" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="17">
+      <c r="A8" s="128">
+        <v>10</v>
+      </c>
+      <c r="B8" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="97" t="s">
+        <v>192</v>
+      </c>
+      <c r="D8" s="29"/>
+      <c r="E8" s="21">
+        <v>10</v>
+      </c>
+      <c r="F8" s="68" t="s">
+        <v>615</v>
+      </c>
+      <c r="G8" s="52" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="17">
+      <c r="A9" s="128">
+        <v>11</v>
+      </c>
+      <c r="B9" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="97" t="s">
+        <v>192</v>
+      </c>
+      <c r="D9" s="29"/>
+      <c r="E9" s="21">
+        <v>11</v>
+      </c>
+      <c r="F9" s="68" t="s">
+        <v>614</v>
+      </c>
+      <c r="G9" s="52" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="17">
+      <c r="A10" s="128">
+        <v>12</v>
+      </c>
+      <c r="B10" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="97" t="s">
+        <v>192</v>
+      </c>
+      <c r="D10" s="29"/>
+      <c r="E10" s="21">
+        <v>12</v>
+      </c>
+      <c r="F10" s="68" t="s">
+        <v>613</v>
+      </c>
+      <c r="G10" s="52" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="18" thickBot="1">
+      <c r="A11" s="129">
+        <v>13</v>
+      </c>
+      <c r="B11" s="46" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" s="135" t="s">
+        <v>192</v>
+      </c>
+      <c r="D11" s="46"/>
+      <c r="E11" s="25">
+        <v>13</v>
+      </c>
+      <c r="F11" s="71" t="s">
+        <v>612</v>
+      </c>
+      <c r="G11" s="130" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="17">
+      <c r="A12" s="127">
+        <v>14</v>
+      </c>
+      <c r="B12" s="33" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" s="132" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12" s="33"/>
+      <c r="E12" s="24">
+        <v>1</v>
+      </c>
+      <c r="F12" s="70" t="s">
+        <v>611</v>
+      </c>
+      <c r="G12" s="51" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="17">
+      <c r="A13" s="128">
+        <v>15</v>
+      </c>
+      <c r="B13" s="29" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" s="97" t="s">
+        <v>26</v>
+      </c>
+      <c r="D13" s="29"/>
+      <c r="E13" s="21">
+        <v>2</v>
+      </c>
+      <c r="F13" s="68" t="s">
+        <v>610</v>
+      </c>
+      <c r="G13" s="52" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="17">
+      <c r="A14" s="128">
+        <v>17</v>
+      </c>
+      <c r="B14" s="29" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" s="34" t="s">
+        <v>36</v>
+      </c>
+      <c r="D14" s="29"/>
+      <c r="E14" s="21">
+        <v>4</v>
+      </c>
+      <c r="F14" s="68" t="s">
+        <v>609</v>
+      </c>
+      <c r="G14" s="52" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="17">
+      <c r="A15" s="128">
+        <v>18</v>
+      </c>
+      <c r="B15" s="29" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" s="97" t="s">
+        <v>26</v>
+      </c>
+      <c r="D15" s="29"/>
+      <c r="E15" s="21">
+        <v>5</v>
+      </c>
+      <c r="F15" s="68" t="s">
+        <v>608</v>
+      </c>
+      <c r="G15" s="52" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="17">
+      <c r="A16" s="128">
+        <v>19</v>
+      </c>
+      <c r="B16" s="29" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16" s="97" t="s">
+        <v>26</v>
+      </c>
+      <c r="D16" s="29"/>
+      <c r="E16" s="21">
+        <v>6</v>
+      </c>
+      <c r="F16" s="68" t="s">
+        <v>607</v>
+      </c>
+      <c r="G16" s="52" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="17">
+      <c r="A17" s="128">
+        <v>20</v>
+      </c>
+      <c r="B17" s="29" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17" s="97" t="s">
+        <v>26</v>
+      </c>
+      <c r="D17" s="29"/>
+      <c r="E17" s="21">
+        <v>7</v>
+      </c>
+      <c r="F17" s="68" t="s">
+        <v>606</v>
+      </c>
+      <c r="G17" s="52" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="17">
+      <c r="A18" s="128">
+        <v>21</v>
+      </c>
+      <c r="B18" s="29" t="s">
+        <v>25</v>
+      </c>
+      <c r="C18" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="D18" s="29"/>
+      <c r="E18" s="21">
+        <v>8</v>
+      </c>
+      <c r="F18" s="68" t="s">
+        <v>605</v>
+      </c>
+      <c r="G18" s="52" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="17">
+      <c r="A19" s="128">
+        <v>23</v>
+      </c>
+      <c r="B19" s="29" t="s">
+        <v>25</v>
+      </c>
+      <c r="C19" s="34" t="s">
+        <v>33</v>
+      </c>
+      <c r="D19" s="29"/>
+      <c r="E19" s="21">
+        <v>10</v>
+      </c>
+      <c r="F19" s="68" t="s">
+        <v>604</v>
+      </c>
+      <c r="G19" s="52" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="17">
+      <c r="A20" s="128">
+        <v>25</v>
+      </c>
+      <c r="B20" s="29" t="s">
+        <v>25</v>
+      </c>
+      <c r="C20" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="D20" s="29"/>
+      <c r="E20" s="21">
+        <v>12</v>
+      </c>
+      <c r="F20" s="68" t="s">
+        <v>603</v>
+      </c>
+      <c r="G20" s="49" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="18" thickBot="1">
+      <c r="A21" s="129">
+        <v>26</v>
+      </c>
+      <c r="B21" s="113" t="s">
+        <v>25</v>
+      </c>
+      <c r="C21" s="114" t="s">
+        <v>26</v>
+      </c>
+      <c r="D21" s="115"/>
+      <c r="E21" s="140">
+        <v>13</v>
+      </c>
+      <c r="F21" s="139" t="s">
+        <v>602</v>
+      </c>
+      <c r="G21" s="53" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="17">
+      <c r="A22" s="127">
+        <v>27</v>
+      </c>
+      <c r="B22" s="33" t="s">
+        <v>44</v>
+      </c>
+      <c r="C22" s="132" t="s">
+        <v>26</v>
+      </c>
+      <c r="D22" s="33"/>
+      <c r="E22" s="24">
+        <v>1</v>
+      </c>
+      <c r="F22" s="70" t="s">
+        <v>601</v>
+      </c>
+      <c r="G22" s="51" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="17">
+      <c r="A23" s="128">
+        <v>28</v>
+      </c>
+      <c r="B23" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="C23" s="97" t="s">
+        <v>26</v>
+      </c>
+      <c r="D23" s="29"/>
+      <c r="E23" s="21">
+        <v>2</v>
+      </c>
+      <c r="F23" s="68" t="s">
+        <v>600</v>
+      </c>
+      <c r="G23" s="138" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="17">
+      <c r="A24" s="128">
+        <v>30</v>
+      </c>
+      <c r="B24" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="C24" s="97" t="s">
+        <v>26</v>
+      </c>
+      <c r="D24" s="29"/>
+      <c r="E24" s="21">
+        <v>4</v>
+      </c>
+      <c r="F24" s="68" t="s">
+        <v>599</v>
+      </c>
+      <c r="G24" s="52" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="17">
+      <c r="A25" s="128">
+        <v>31</v>
+      </c>
+      <c r="B25" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="C25" s="97" t="s">
+        <v>26</v>
+      </c>
+      <c r="D25" s="29"/>
+      <c r="E25" s="21">
+        <v>5</v>
+      </c>
+      <c r="F25" s="68" t="s">
+        <v>598</v>
+      </c>
+      <c r="G25" s="52" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="17">
+      <c r="A26" s="128">
+        <v>32</v>
+      </c>
+      <c r="B26" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="C26" s="34" t="s">
+        <v>28</v>
+      </c>
+      <c r="D26" s="29"/>
+      <c r="E26" s="21">
+        <v>6</v>
+      </c>
+      <c r="F26" s="68" t="s">
+        <v>597</v>
+      </c>
+      <c r="G26" s="52" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="17">
+      <c r="A27" s="128">
+        <v>33</v>
+      </c>
+      <c r="B27" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="C27" s="34" t="s">
+        <v>26</v>
+      </c>
+      <c r="D27" s="29"/>
+      <c r="E27" s="21">
+        <v>7</v>
+      </c>
+      <c r="F27" s="68" t="s">
+        <v>596</v>
+      </c>
+      <c r="G27" s="111" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="17">
+      <c r="A28" s="128">
+        <v>34</v>
+      </c>
+      <c r="B28" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="C28" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="D28" s="29"/>
+      <c r="E28" s="21">
+        <v>8</v>
+      </c>
+      <c r="F28" s="68" t="s">
+        <v>595</v>
+      </c>
+      <c r="G28" s="52" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="17">
+      <c r="A29" s="128">
+        <v>35</v>
+      </c>
+      <c r="B29" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="C29" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="D29" s="29"/>
+      <c r="E29" s="21">
+        <v>9</v>
+      </c>
+      <c r="F29" s="68" t="s">
+        <v>594</v>
+      </c>
+      <c r="G29" s="52" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="17">
+      <c r="A30" s="128">
+        <v>37</v>
+      </c>
+      <c r="B30" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="C30" s="97" t="s">
+        <v>26</v>
+      </c>
+      <c r="D30" s="29"/>
+      <c r="E30" s="21">
+        <v>11</v>
+      </c>
+      <c r="F30" s="68" t="s">
+        <v>593</v>
+      </c>
+      <c r="G30" s="52" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="18" thickBot="1">
+      <c r="A31" s="129">
+        <v>39</v>
+      </c>
+      <c r="B31" s="113" t="s">
+        <v>44</v>
+      </c>
+      <c r="C31" s="114" t="s">
+        <v>26</v>
+      </c>
+      <c r="D31" s="115"/>
+      <c r="E31" s="116">
+        <v>13</v>
+      </c>
+      <c r="F31" s="117" t="s">
+        <v>592</v>
+      </c>
+      <c r="G31" s="53" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="17">
+      <c r="A32" s="127">
+        <v>41</v>
+      </c>
+      <c r="B32" s="33" t="s">
+        <v>58</v>
+      </c>
+      <c r="C32" s="132" t="s">
+        <v>26</v>
+      </c>
+      <c r="D32" s="33"/>
+      <c r="E32" s="24">
+        <v>2</v>
+      </c>
+      <c r="F32" s="70" t="s">
+        <v>591</v>
+      </c>
+      <c r="G32" s="51" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="17">
+      <c r="A33" s="128">
+        <v>43</v>
+      </c>
+      <c r="B33" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="C33" s="97" t="s">
+        <v>26</v>
+      </c>
+      <c r="D33" s="29"/>
+      <c r="E33" s="21">
+        <v>4</v>
+      </c>
+      <c r="F33" s="68" t="s">
+        <v>590</v>
+      </c>
+      <c r="G33" s="52" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="17">
+      <c r="A34" s="128">
+        <v>45</v>
+      </c>
+      <c r="B34" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="C34" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="D34" s="29"/>
+      <c r="E34" s="21">
+        <v>6</v>
+      </c>
+      <c r="F34" s="68" t="s">
+        <v>589</v>
+      </c>
+      <c r="G34" s="49" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="17">
+      <c r="A35" s="128">
+        <v>46</v>
+      </c>
+      <c r="B35" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="C35" s="97" t="s">
+        <v>26</v>
+      </c>
+      <c r="D35" s="29"/>
+      <c r="E35" s="21">
+        <v>7</v>
+      </c>
+      <c r="F35" s="68" t="s">
+        <v>588</v>
+      </c>
+      <c r="G35" s="52" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="17">
+      <c r="A36" s="128">
+        <v>47</v>
+      </c>
+      <c r="B36" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="C36" s="97" t="s">
+        <v>26</v>
+      </c>
+      <c r="D36" s="29"/>
+      <c r="E36" s="21">
+        <v>8</v>
+      </c>
+      <c r="F36" s="68" t="s">
+        <v>587</v>
+      </c>
+      <c r="G36" s="52" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="34">
+      <c r="A37" s="128">
+        <v>48</v>
+      </c>
+      <c r="B37" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="C37" s="34" t="s">
+        <v>36</v>
+      </c>
+      <c r="D37" s="29"/>
+      <c r="E37" s="21">
+        <v>9</v>
+      </c>
+      <c r="F37" s="68" t="s">
+        <v>586</v>
+      </c>
+      <c r="G37" s="52" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" ht="17">
+      <c r="A38" s="128">
+        <v>49</v>
+      </c>
+      <c r="B38" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="C38" s="97" t="s">
+        <v>26</v>
+      </c>
+      <c r="D38" s="29"/>
+      <c r="E38" s="21">
+        <v>10</v>
+      </c>
+      <c r="F38" s="68" t="s">
+        <v>585</v>
+      </c>
+      <c r="G38" s="52" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" ht="17">
+      <c r="A39" s="128">
+        <v>50</v>
+      </c>
+      <c r="B39" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="C39" s="97" t="s">
+        <v>26</v>
+      </c>
+      <c r="D39" s="29"/>
+      <c r="E39" s="21">
+        <v>11</v>
+      </c>
+      <c r="F39" s="68" t="s">
+        <v>584</v>
+      </c>
+      <c r="G39" s="52" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" ht="17">
+      <c r="A40" s="128">
+        <v>51</v>
+      </c>
+      <c r="B40" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="C40" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="D40" s="29"/>
+      <c r="E40" s="21">
+        <v>12</v>
+      </c>
+      <c r="F40" s="68" t="s">
+        <v>583</v>
+      </c>
+      <c r="G40" s="49" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" ht="18" thickBot="1">
+      <c r="A41" s="129">
+        <v>54</v>
+      </c>
+      <c r="B41" s="46" t="s">
+        <v>58</v>
+      </c>
+      <c r="C41" s="36" t="s">
+        <v>39</v>
+      </c>
+      <c r="D41" s="46"/>
+      <c r="E41" s="25">
+        <v>15</v>
+      </c>
+      <c r="F41" s="71" t="s">
+        <v>582</v>
+      </c>
+      <c r="G41" s="130" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="17">
+      <c r="A42" s="127">
+        <v>55</v>
+      </c>
+      <c r="B42" s="33" t="s">
+        <v>74</v>
+      </c>
+      <c r="C42" s="132" t="s">
+        <v>26</v>
+      </c>
+      <c r="D42" s="78" t="s">
+        <v>75</v>
+      </c>
+      <c r="E42" s="24">
+        <v>1</v>
+      </c>
+      <c r="F42" s="70" t="s">
+        <v>581</v>
+      </c>
+      <c r="G42" s="51" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" ht="17">
+      <c r="A43" s="128">
+        <v>56</v>
+      </c>
+      <c r="B43" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="C43" s="97" t="s">
+        <v>26</v>
+      </c>
+      <c r="D43" s="77" t="s">
+        <v>75</v>
+      </c>
+      <c r="E43" s="21">
+        <v>2</v>
+      </c>
+      <c r="F43" s="68" t="s">
+        <v>580</v>
+      </c>
+      <c r="G43" s="52" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" ht="17">
+      <c r="A44" s="128">
+        <v>57</v>
+      </c>
+      <c r="B44" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="C44" s="97" t="s">
+        <v>26</v>
+      </c>
+      <c r="D44" s="77" t="s">
+        <v>75</v>
+      </c>
+      <c r="E44" s="21">
+        <v>3</v>
+      </c>
+      <c r="F44" s="68" t="s">
+        <v>579</v>
+      </c>
+      <c r="G44" s="52" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" ht="17">
+      <c r="A45" s="128">
+        <v>60</v>
+      </c>
+      <c r="B45" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="C45" s="97" t="s">
+        <v>26</v>
+      </c>
+      <c r="D45" s="77" t="s">
+        <v>75</v>
+      </c>
+      <c r="E45" s="21">
+        <v>6</v>
+      </c>
+      <c r="F45" s="68" t="s">
+        <v>578</v>
+      </c>
+      <c r="G45" s="52" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" ht="17">
+      <c r="A46" s="128">
+        <v>62</v>
+      </c>
+      <c r="B46" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="C46" s="97" t="s">
+        <v>26</v>
+      </c>
+      <c r="D46" s="77" t="s">
+        <v>75</v>
+      </c>
+      <c r="E46" s="21">
+        <v>8</v>
+      </c>
+      <c r="F46" s="68" t="s">
+        <v>577</v>
+      </c>
+      <c r="G46" s="52" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" ht="17">
+      <c r="A47" s="128">
+        <v>65</v>
+      </c>
+      <c r="B47" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="C47" s="97" t="s">
+        <v>26</v>
+      </c>
+      <c r="D47" s="77" t="s">
+        <v>75</v>
+      </c>
+      <c r="E47" s="21">
+        <v>11</v>
+      </c>
+      <c r="F47" s="68" t="s">
+        <v>576</v>
+      </c>
+      <c r="G47" s="52" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" ht="17">
+      <c r="A48" s="128">
+        <v>66</v>
+      </c>
+      <c r="B48" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="C48" s="34" t="s">
+        <v>36</v>
+      </c>
+      <c r="D48" s="77" t="s">
+        <v>83</v>
+      </c>
+      <c r="E48" s="21">
+        <v>12</v>
+      </c>
+      <c r="F48" s="68" t="s">
+        <v>575</v>
+      </c>
+      <c r="G48" s="52" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" ht="17">
+      <c r="A49" s="128">
+        <v>67</v>
+      </c>
+      <c r="B49" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="C49" s="97" t="s">
+        <v>26</v>
+      </c>
+      <c r="D49" s="77" t="s">
+        <v>83</v>
+      </c>
+      <c r="E49" s="21">
+        <v>13</v>
+      </c>
+      <c r="F49" s="68" t="s">
+        <v>574</v>
+      </c>
+      <c r="G49" s="52" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" ht="17">
+      <c r="A50" s="128">
+        <v>68</v>
+      </c>
+      <c r="B50" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="C50" s="34" t="s">
+        <v>28</v>
+      </c>
+      <c r="D50" s="77" t="s">
+        <v>83</v>
+      </c>
+      <c r="E50" s="21">
+        <v>14</v>
+      </c>
+      <c r="F50" s="68" t="s">
+        <v>573</v>
+      </c>
+      <c r="G50" s="52" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" ht="18" thickBot="1">
+      <c r="A51" s="129">
+        <v>69</v>
+      </c>
+      <c r="B51" s="46" t="s">
+        <v>74</v>
+      </c>
+      <c r="C51" s="36" t="s">
+        <v>39</v>
+      </c>
+      <c r="D51" s="126" t="s">
+        <v>83</v>
+      </c>
+      <c r="E51" s="25">
+        <v>15</v>
+      </c>
+      <c r="F51" s="71" t="s">
+        <v>572</v>
+      </c>
+      <c r="G51" s="130" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" ht="17">
+      <c r="A52" s="127">
+        <v>71</v>
+      </c>
+      <c r="B52" s="33" t="s">
+        <v>90</v>
+      </c>
+      <c r="C52" s="43" t="s">
+        <v>39</v>
+      </c>
+      <c r="D52" s="33"/>
+      <c r="E52" s="24">
+        <v>2</v>
+      </c>
+      <c r="F52" s="70" t="s">
+        <v>571</v>
+      </c>
+      <c r="G52" s="51" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" ht="17">
+      <c r="A53" s="128">
+        <v>72</v>
+      </c>
+      <c r="B53" s="29" t="s">
+        <v>90</v>
+      </c>
+      <c r="C53" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="D53" s="29"/>
+      <c r="E53" s="21">
+        <v>3</v>
+      </c>
+      <c r="F53" s="68" t="s">
+        <v>570</v>
+      </c>
+      <c r="G53" s="52" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" s="5" customFormat="1" ht="17">
+      <c r="A54" s="128">
+        <v>73</v>
+      </c>
+      <c r="B54" s="29" t="s">
+        <v>90</v>
+      </c>
+      <c r="C54" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="D54" s="29"/>
+      <c r="E54" s="21">
+        <v>4</v>
+      </c>
+      <c r="F54" s="68" t="s">
+        <v>569</v>
+      </c>
+      <c r="G54" s="52" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" ht="17">
+      <c r="A55" s="128">
+        <v>74</v>
+      </c>
+      <c r="B55" s="29" t="s">
+        <v>90</v>
+      </c>
+      <c r="C55" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="D55" s="29"/>
+      <c r="E55" s="21">
+        <v>5</v>
+      </c>
+      <c r="F55" s="68" t="s">
+        <v>568</v>
+      </c>
+      <c r="G55" s="52" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" ht="17">
+      <c r="A56" s="128">
+        <v>75</v>
+      </c>
+      <c r="B56" s="29" t="s">
+        <v>90</v>
+      </c>
+      <c r="C56" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="D56" s="29"/>
+      <c r="E56" s="21">
+        <v>6</v>
+      </c>
+      <c r="F56" s="68" t="s">
+        <v>567</v>
+      </c>
+      <c r="G56" s="52" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" ht="17">
+      <c r="A57" s="128">
+        <v>76</v>
+      </c>
+      <c r="B57" s="29" t="s">
+        <v>90</v>
+      </c>
+      <c r="C57" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="D57" s="29"/>
+      <c r="E57" s="21">
+        <v>7</v>
+      </c>
+      <c r="F57" s="68" t="s">
+        <v>566</v>
+      </c>
+      <c r="G57" s="52" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" ht="17">
+      <c r="A58" s="128">
+        <v>77</v>
+      </c>
+      <c r="B58" s="29" t="s">
+        <v>90</v>
+      </c>
+      <c r="C58" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="D58" s="29"/>
+      <c r="E58" s="21">
+        <v>8</v>
+      </c>
+      <c r="F58" s="68" t="s">
+        <v>565</v>
+      </c>
+      <c r="G58" s="52" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" ht="17">
+      <c r="A59" s="128">
+        <v>78</v>
+      </c>
+      <c r="B59" s="29" t="s">
+        <v>90</v>
+      </c>
+      <c r="C59" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="D59" s="29"/>
+      <c r="E59" s="21">
+        <v>9</v>
+      </c>
+      <c r="F59" s="68" t="s">
+        <v>564</v>
+      </c>
+      <c r="G59" s="52" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" ht="17">
+      <c r="A60" s="128">
+        <v>79</v>
+      </c>
+      <c r="B60" s="29" t="s">
+        <v>90</v>
+      </c>
+      <c r="C60" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="D60" s="29"/>
+      <c r="E60" s="21">
+        <v>10</v>
+      </c>
+      <c r="F60" s="68" t="s">
+        <v>563</v>
+      </c>
+      <c r="G60" s="52" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" ht="18" thickBot="1">
+      <c r="A61" s="129">
+        <v>81</v>
+      </c>
+      <c r="B61" s="46" t="s">
+        <v>90</v>
+      </c>
+      <c r="C61" s="36" t="s">
+        <v>39</v>
+      </c>
+      <c r="D61" s="46"/>
+      <c r="E61" s="25">
+        <v>12</v>
+      </c>
+      <c r="F61" s="71" t="s">
+        <v>562</v>
+      </c>
+      <c r="G61" s="130" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" ht="17">
+      <c r="A62" s="127">
+        <v>83</v>
+      </c>
+      <c r="B62" s="33" t="s">
+        <v>103</v>
+      </c>
+      <c r="C62" s="43" t="s">
+        <v>26</v>
+      </c>
+      <c r="D62" s="33"/>
+      <c r="E62" s="24">
+        <v>1</v>
+      </c>
+      <c r="F62" s="70" t="s">
+        <v>561</v>
+      </c>
+      <c r="G62" s="51" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" ht="34">
+      <c r="A63" s="128">
+        <v>85</v>
+      </c>
+      <c r="B63" s="29" t="s">
+        <v>103</v>
+      </c>
+      <c r="C63" s="97" t="s">
+        <v>26</v>
+      </c>
+      <c r="D63" s="29"/>
+      <c r="E63" s="21">
+        <v>3</v>
+      </c>
+      <c r="F63" s="68" t="s">
+        <v>560</v>
+      </c>
+      <c r="G63" s="49" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" ht="17">
+      <c r="A64" s="128">
+        <v>86</v>
+      </c>
+      <c r="B64" s="29" t="s">
+        <v>103</v>
+      </c>
+      <c r="C64" s="97" t="s">
+        <v>26</v>
+      </c>
+      <c r="D64" s="29"/>
+      <c r="E64" s="21">
+        <v>4</v>
+      </c>
+      <c r="F64" s="68" t="s">
+        <v>559</v>
+      </c>
+      <c r="G64" s="52" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" ht="17">
+      <c r="A65" s="128">
+        <v>87</v>
+      </c>
+      <c r="B65" s="29" t="s">
+        <v>103</v>
+      </c>
+      <c r="C65" s="34" t="s">
+        <v>105</v>
+      </c>
+      <c r="D65" s="29"/>
+      <c r="E65" s="21">
+        <v>5</v>
+      </c>
+      <c r="F65" s="68" t="s">
+        <v>558</v>
+      </c>
+      <c r="G65" s="49" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" ht="17">
+      <c r="A66" s="128">
+        <v>89</v>
+      </c>
+      <c r="B66" s="29" t="s">
+        <v>103</v>
+      </c>
+      <c r="C66" s="97" t="s">
+        <v>26</v>
+      </c>
+      <c r="D66" s="29"/>
+      <c r="E66" s="21">
+        <v>7</v>
+      </c>
+      <c r="F66" s="68" t="s">
+        <v>557</v>
+      </c>
+      <c r="G66" s="52" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" ht="17">
+      <c r="A67" s="128">
+        <v>91</v>
+      </c>
+      <c r="B67" s="29" t="s">
+        <v>103</v>
+      </c>
+      <c r="C67" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="D67" s="29"/>
+      <c r="E67" s="21">
+        <v>9</v>
+      </c>
+      <c r="F67" s="68" t="s">
+        <v>556</v>
+      </c>
+      <c r="G67" s="52" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" ht="17">
+      <c r="A68" s="128">
+        <v>92</v>
+      </c>
+      <c r="B68" s="29" t="s">
+        <v>103</v>
+      </c>
+      <c r="C68" s="34" t="s">
+        <v>28</v>
+      </c>
+      <c r="D68" s="29"/>
+      <c r="E68" s="21">
+        <v>10</v>
+      </c>
+      <c r="F68" s="68" t="s">
+        <v>555</v>
+      </c>
+      <c r="G68" s="52" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" ht="17">
+      <c r="A69" s="128">
+        <v>93</v>
+      </c>
+      <c r="B69" s="29" t="s">
+        <v>103</v>
+      </c>
+      <c r="C69" s="34" t="s">
+        <v>28</v>
+      </c>
+      <c r="D69" s="29"/>
+      <c r="E69" s="21">
+        <v>11</v>
+      </c>
+      <c r="F69" s="68" t="s">
+        <v>554</v>
+      </c>
+      <c r="G69" s="52" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" ht="17">
+      <c r="A70" s="128">
+        <v>94</v>
+      </c>
+      <c r="B70" s="29" t="s">
+        <v>103</v>
+      </c>
+      <c r="C70" s="34" t="s">
+        <v>105</v>
+      </c>
+      <c r="D70" s="29"/>
+      <c r="E70" s="21">
+        <v>12</v>
+      </c>
+      <c r="F70" s="68" t="s">
+        <v>553</v>
+      </c>
+      <c r="G70" s="52" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" ht="18" thickBot="1">
+      <c r="A71" s="129">
+        <v>95</v>
+      </c>
+      <c r="B71" s="113" t="s">
+        <v>103</v>
+      </c>
+      <c r="C71" s="114" t="s">
+        <v>26</v>
+      </c>
+      <c r="D71" s="115"/>
+      <c r="E71" s="116">
+        <v>13</v>
+      </c>
+      <c r="F71" s="117" t="s">
+        <v>552</v>
+      </c>
+      <c r="G71" s="53" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" ht="17">
+      <c r="A72" s="127">
+        <v>96</v>
+      </c>
+      <c r="B72" s="33" t="s">
+        <v>121</v>
+      </c>
+      <c r="C72" s="132" t="s">
+        <v>129</v>
+      </c>
+      <c r="D72" s="33"/>
+      <c r="E72" s="24">
+        <v>1</v>
+      </c>
+      <c r="F72" s="70" t="s">
+        <v>551</v>
+      </c>
+      <c r="G72" s="51" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" ht="17">
+      <c r="A73" s="128">
+        <v>97</v>
+      </c>
+      <c r="B73" s="29" t="s">
+        <v>121</v>
+      </c>
+      <c r="C73" s="97" t="s">
+        <v>129</v>
+      </c>
+      <c r="D73" s="29"/>
+      <c r="E73" s="21">
+        <v>2</v>
+      </c>
+      <c r="F73" s="68" t="s">
+        <v>550</v>
+      </c>
+      <c r="G73" s="52" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" ht="17">
+      <c r="A74" s="128">
+        <v>98</v>
+      </c>
+      <c r="B74" s="29" t="s">
+        <v>121</v>
+      </c>
+      <c r="C74" s="97" t="s">
+        <v>129</v>
+      </c>
+      <c r="D74" s="29"/>
+      <c r="E74" s="21">
+        <v>3</v>
+      </c>
+      <c r="F74" s="68" t="s">
+        <v>549</v>
+      </c>
+      <c r="G74" s="52" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" ht="17">
+      <c r="A75" s="128">
+        <v>100</v>
+      </c>
+      <c r="B75" s="29" t="s">
+        <v>121</v>
+      </c>
+      <c r="C75" s="97" t="s">
+        <v>122</v>
+      </c>
+      <c r="D75" s="29"/>
+      <c r="E75" s="21">
+        <v>5</v>
+      </c>
+      <c r="F75" s="68" t="s">
+        <v>548</v>
+      </c>
+      <c r="G75" s="52" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" ht="17">
+      <c r="A76" s="128">
+        <v>101</v>
+      </c>
+      <c r="B76" s="29" t="s">
+        <v>121</v>
+      </c>
+      <c r="C76" s="97" t="s">
+        <v>122</v>
+      </c>
+      <c r="D76" s="29"/>
+      <c r="E76" s="21">
+        <v>6</v>
+      </c>
+      <c r="F76" s="68" t="s">
+        <v>547</v>
+      </c>
+      <c r="G76" s="52" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" ht="17">
+      <c r="A77" s="128">
+        <v>103</v>
+      </c>
+      <c r="B77" s="29" t="s">
+        <v>121</v>
+      </c>
+      <c r="C77" s="97" t="s">
+        <v>129</v>
+      </c>
+      <c r="D77" s="29"/>
+      <c r="E77" s="21">
+        <v>8</v>
+      </c>
+      <c r="F77" s="68" t="s">
+        <v>546</v>
+      </c>
+      <c r="G77" s="49" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" ht="17">
+      <c r="A78" s="128">
+        <v>105</v>
+      </c>
+      <c r="B78" s="29" t="s">
+        <v>121</v>
+      </c>
+      <c r="C78" s="97" t="s">
+        <v>129</v>
+      </c>
+      <c r="D78" s="29"/>
+      <c r="E78" s="21">
+        <v>10</v>
+      </c>
+      <c r="F78" s="68" t="s">
+        <v>545</v>
+      </c>
+      <c r="G78" s="52" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" ht="17">
+      <c r="A79" s="128">
+        <v>106</v>
+      </c>
+      <c r="B79" s="29" t="s">
+        <v>121</v>
+      </c>
+      <c r="C79" s="97" t="s">
+        <v>129</v>
+      </c>
+      <c r="D79" s="29"/>
+      <c r="E79" s="21">
+        <v>11</v>
+      </c>
+      <c r="F79" s="68" t="s">
+        <v>544</v>
+      </c>
+      <c r="G79" s="52" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" ht="17">
+      <c r="A80" s="128">
+        <v>107</v>
+      </c>
+      <c r="B80" s="29" t="s">
+        <v>121</v>
+      </c>
+      <c r="C80" s="97" t="s">
+        <v>129</v>
+      </c>
+      <c r="D80" s="29"/>
+      <c r="E80" s="21">
+        <v>12</v>
+      </c>
+      <c r="F80" s="68" t="s">
+        <v>543</v>
+      </c>
+      <c r="G80" s="52" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" ht="18" thickBot="1">
+      <c r="A81" s="129">
+        <v>108</v>
+      </c>
+      <c r="B81" s="113" t="s">
+        <v>121</v>
+      </c>
+      <c r="C81" s="114" t="s">
+        <v>129</v>
+      </c>
+      <c r="D81" s="115"/>
+      <c r="E81" s="116">
+        <v>13</v>
+      </c>
+      <c r="F81" s="117" t="s">
+        <v>542</v>
+      </c>
+      <c r="G81" s="53" t="s">
+        <v>293</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="68" fitToHeight="4" orientation="landscape" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -8027,9 +10049,9 @@
     <sortCondition sortBy="cellColor" ref="G2:G109" dxfId="0"/>
   </sortState>
   <customSheetViews>
-    <customSheetView guid="{3D544592-D893-4912-8A4C-A9212B9C1328}" fitToPage="1">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="L1" sqref="G1:L1048576"/>
+    <customSheetView guid="{E395C88E-3BA8-B344-A1BC-A46BF8755BD3}" fitToPage="1" hiddenColumns="1">
+      <pane ySplit="1" topLeftCell="A46" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="H109" sqref="H109"/>
       <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
       <pageSetup scale="68" fitToHeight="4" orientation="landscape" r:id="rId1"/>
     </customSheetView>
@@ -8044,27 +10066,27 @@
         </sortState>
       </autoFilter>
     </customSheetView>
-    <customSheetView guid="{E395C88E-3BA8-B344-A1BC-A46BF8755BD3}" fitToPage="1" hiddenColumns="1">
-      <pane ySplit="1" topLeftCell="A46" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="H109" sqref="H109"/>
+    <customSheetView guid="{3D544592-D893-4912-8A4C-A9212B9C1328}" fitToPage="1">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="L1" sqref="G1:L1048576"/>
       <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
       <pageSetup scale="68" fitToHeight="4" orientation="landscape" r:id="rId3"/>
     </customSheetView>
   </customSheetViews>
-  <phoneticPr fontId="7" type="noConversion"/>
+  <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="68" fitToHeight="4" orientation="landscape" r:id="rId4"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F981DB43-5CB2-2645-B4A1-50D990218B29}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:G81"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="75" workbookViewId="0">
+    <sheetView zoomScale="200" zoomScaleNormal="75" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
       <selection pane="bottomLeft" activeCell="F2" sqref="F2:F81"/>
     </sheetView>
@@ -9822,7 +11844,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A2:G100"/>
   <sheetViews>
@@ -11881,7 +13903,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F303D1AF-32B3-D847-988A-41E7647C4224}">
   <dimension ref="A1:D80"/>
   <sheetViews>

</xml_diff>